<commit_message>
Changes to the signal creating files.
</commit_message>
<xml_diff>
--- a/SIB/signals_simulation/Caclulation_example_for_simulations_dontdelete.xlsx
+++ b/SIB/signals_simulation/Caclulation_example_for_simulations_dontdelete.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>round</t>
   </si>
@@ -101,12 +101,21 @@
   <si>
     <t>Bayesian posterior</t>
   </si>
+  <si>
+    <t>Posterior under SI</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SI-factor on ingroup signals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +156,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -292,13 +309,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -605,19 +624,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="12" max="12" width="27" customWidth="1"/>
-    <col min="13" max="16" width="20.6328125" customWidth="1"/>
+    <col min="13" max="17" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,20 +664,23 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -669,25 +691,25 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>6030</v>
+        <v>617</v>
       </c>
       <c r="E2">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F2">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G2">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H2">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I2">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J2">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>16</v>
@@ -704,8 +726,11 @@
       <c r="P2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -716,47 +741,51 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>6042</v>
+        <v>755</v>
       </c>
       <c r="E3">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F3">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G3">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H3">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I3">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J3">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L3" s="5">
         <v>1</v>
       </c>
       <c r="M3" s="2">
         <f>SUM(D2:D7)/6</f>
-        <v>6038</v>
+        <v>606.5</v>
       </c>
       <c r="N3" s="2">
         <f>(SUM(D2:D4)+MAX(D5:D7))/4</f>
-        <v>6038.5</v>
+        <v>630.25</v>
       </c>
       <c r="O3" s="2">
         <f>(SUM(D2:D5)+AVERAGE(D5,D6)+AVERAGE(D5,D7))/6</f>
-        <v>6039.5</v>
+        <v>613.83333333333337</v>
       </c>
       <c r="P3" s="2">
         <f>(SUM(D2:D7) + P15*D8)/7</f>
-        <v>6080.6785714285716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>624.82857142857142</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>(SUM(D2:D4)*Q15 + SUM(D5:D7)*(1/Q15))/6</f>
+        <v>612.39090909090908</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -767,47 +796,51 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>6033</v>
+        <v>546</v>
       </c>
       <c r="E4">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F4">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G4">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H4">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I4">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J4">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L4" s="6">
         <v>2</v>
       </c>
       <c r="M4" s="2">
         <f>SUM(D9:D14)/6</f>
-        <v>3347.1666666666665</v>
+        <v>620.16666666666663</v>
       </c>
       <c r="N4" s="2">
         <f>(SUM(D9:D11)+MAX(D12:D14))/4</f>
-        <v>3347.75</v>
+        <v>648.75</v>
       </c>
       <c r="O4" s="2">
         <f>(SUM(D9:D12)+AVERAGE(D12,D13)+AVERAGE(D12,D14))/6</f>
-        <v>3348.8333333333335</v>
+        <v>624.33333333333337</v>
       </c>
       <c r="P4" s="2">
         <f>(SUM(D9:D14) + P15*D15)/7</f>
-        <v>3371.9500000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>615.17142857142858</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>(SUM(D9:D11)*Q15 + SUM(D12:D14)*(1/Q15))/6</f>
+        <v>626.21515151515155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -818,47 +851,51 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>6047</v>
+        <v>603</v>
       </c>
       <c r="E5">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F5">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G5">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H5">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I5">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J5">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L5" s="6">
         <v>3</v>
       </c>
       <c r="M5" s="2">
         <f>SUM(D16:D21)/6</f>
-        <v>4014.1666666666665</v>
+        <v>354.5</v>
       </c>
       <c r="N5" s="2">
         <f>(SUM(D16:D18)+MAX(D19:D21))/4</f>
-        <v>4017.75</v>
+        <v>345.25</v>
       </c>
       <c r="O5" s="2">
         <f>(SUM(D16:D19)+AVERAGE(D19,D20)+AVERAGE(D19,D21))/6</f>
-        <v>4016</v>
+        <v>359.66666666666669</v>
       </c>
       <c r="P5" s="2">
         <f>(SUM(D16:D21) + P15*D22)/7</f>
-        <v>4043.5642857142857</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>338.2714285714286</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>(SUM(D16:D18)*Q15 + SUM(D19:D21)*(1/Q15))/6</f>
+        <v>353.35909090909098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -869,47 +906,51 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>6049</v>
+        <v>569</v>
       </c>
       <c r="E6">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F6">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G6">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H6">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I6">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J6">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L6" s="6">
         <v>4</v>
       </c>
       <c r="M6" s="2">
         <f>SUM(D23:D28)/6</f>
-        <v>9098.1666666666661</v>
+        <v>100</v>
       </c>
       <c r="N6" s="2">
         <f>(SUM(D23:D25)+MAX(D26:D28))/4</f>
-        <v>9100.25</v>
+        <v>132.5</v>
       </c>
       <c r="O6" s="2">
         <f>(SUM(D23:D26)+AVERAGE(D26,D27)+AVERAGE(D26,D28))/6</f>
-        <v>9101.1666666666661</v>
+        <v>118</v>
       </c>
       <c r="P6" s="2">
         <f>(SUM(D23:D28) + P15*D29)/7</f>
-        <v>9163.7285714285717</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>120.12857142857142</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>(SUM(D23:D25)*Q15 + SUM(D26:D28)*(1/Q15))/6</f>
+        <v>103.22272727272728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -920,47 +961,51 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>6027</v>
+        <v>549</v>
       </c>
       <c r="E7">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F7">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G7">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H7">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I7">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J7">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L7" s="6">
         <v>5</v>
       </c>
       <c r="M7" s="2">
         <f>SUM(D30:D35)/6</f>
-        <v>9078.8333333333339</v>
+        <v>190.5</v>
       </c>
       <c r="N7" s="2">
         <f>(SUM(D30:D32)+MAX(D33:D35))/4</f>
-        <v>9080.75</v>
+        <v>190.75</v>
       </c>
       <c r="O7" s="2">
         <f>(SUM(D30:D33)+AVERAGE(D33,D34)+AVERAGE(D33,D35))/6</f>
-        <v>9080.1666666666661</v>
+        <v>173</v>
       </c>
       <c r="P7" s="2">
         <f>(SUM(D30:D35) + P15*D36)/7</f>
-        <v>9141.6071428571431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+        <v>180.72857142857143</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>(SUM(D30:D32)*Q15 + SUM(D33:D35)*(1/Q15))/6</f>
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -971,47 +1016,51 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>6035</v>
+        <v>668</v>
       </c>
       <c r="E8">
-        <v>6038</v>
+        <v>652</v>
       </c>
       <c r="F8">
-        <v>-6</v>
+        <v>65.666666669999998</v>
       </c>
       <c r="G8">
-        <v>-9</v>
+        <v>-44</v>
       </c>
       <c r="H8">
-        <v>6048</v>
+        <v>586</v>
       </c>
       <c r="I8">
-        <v>6037</v>
+        <v>576</v>
       </c>
       <c r="J8">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L8" s="6">
         <v>6</v>
       </c>
       <c r="M8" s="2">
         <f>SUM(D37:D42)/6</f>
-        <v>2811</v>
+        <v>559</v>
       </c>
       <c r="N8" s="2">
         <f>(SUM(D37:D39)+MAX(D40:D42))/4</f>
-        <v>2815</v>
+        <v>573.5</v>
       </c>
       <c r="O8" s="2">
         <f>(SUM(D37:D40)+AVERAGE(D40,D41)+AVERAGE(D40,D42))/6</f>
-        <v>2813.8333333333335</v>
+        <v>540.66666666666663</v>
       </c>
       <c r="P8" s="2">
         <f>(SUM(D37:D42) + P15*D43)/7</f>
-        <v>2829.8785714285718</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+        <v>552.21428571428567</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>(SUM(D37:D39)*Q15 + SUM(D40:D42)*(1/Q15))/6</f>
+        <v>559.88636363636363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1022,47 +1071,51 @@
         <v>9</v>
       </c>
       <c r="D9">
-        <v>3348</v>
+        <v>685</v>
       </c>
       <c r="E9">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F9">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G9">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H9">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I9">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J9">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L9" s="6">
         <v>7</v>
       </c>
       <c r="M9" s="2">
         <f>SUM(D44:D49)/6</f>
-        <v>9193</v>
+        <v>182.66666666666666</v>
       </c>
       <c r="N9" s="2">
         <f>(SUM(D44:D46)+MAX(D47:D49))/4</f>
-        <v>9194</v>
+        <v>190.5</v>
       </c>
       <c r="O9" s="2">
         <f>(SUM(D44:D47)+AVERAGE(D47,D48)+AVERAGE(D47,D49))/6</f>
-        <v>9194.5</v>
+        <v>151.33333333333334</v>
       </c>
       <c r="P9" s="2">
         <f>(SUM(D44:D49) + P15*D50)/7</f>
-        <v>9259.2642857142855</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+        <v>192.55714285714288</v>
+      </c>
+      <c r="Q9" s="2">
+        <f>(SUM(D44:D46)*Q15 + SUM(D47:D49)*(1/Q15))/6</f>
+        <v>180.85606060606062</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1073,47 +1126,51 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>3340</v>
+        <v>712</v>
       </c>
       <c r="E10">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F10">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G10">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H10">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I10">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J10">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L10" s="6">
         <v>8</v>
       </c>
       <c r="M10" s="2">
         <f>SUM(D51:D56)/6</f>
-        <v>9400.8333333333339</v>
+        <v>100.16666666666667</v>
       </c>
       <c r="N10" s="2">
         <f>(SUM(D51:D53)+MAX(D54:D56))/4</f>
-        <v>9403.75</v>
+        <v>136.25</v>
       </c>
       <c r="O10" s="2">
         <f>(SUM(D51:D54)+AVERAGE(D54,D55)+AVERAGE(D54,D56))/6</f>
-        <v>9399</v>
+        <v>94.166666666666671</v>
       </c>
       <c r="P10" s="2">
         <f>(SUM(E51:E54)+AVERAGE(E54,E55)+AVERAGE(E54,E56))/6</f>
-        <v>9401</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+      <c r="Q10" s="2">
+        <f>(SUM(D51:D53)*Q15 + SUM(D54:D56)*(1/Q15))/6</f>
+        <v>104.64696969696972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1124,47 +1181,51 @@
         <v>11</v>
       </c>
       <c r="D11">
-        <v>3347</v>
+        <v>565</v>
       </c>
       <c r="E11">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F11">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G11">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H11">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I11">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J11">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L11" s="6">
         <v>9</v>
       </c>
       <c r="M11" s="2">
         <f>SUM(D58:D63)/6</f>
-        <v>9967.6666666666661</v>
+        <v>399.5</v>
       </c>
       <c r="N11" s="2">
         <f>(SUM(D58:D60)+MAX(D61:D63))/4</f>
-        <v>9970.5</v>
+        <v>430.25</v>
       </c>
       <c r="O11" s="2">
         <f>(SUM(D58:D61)+AVERAGE(D61,D62)+AVERAGE(D61,D63))/6</f>
-        <v>9966.3333333333339</v>
+        <v>389.5</v>
       </c>
       <c r="P11" s="2">
         <f>(SUM(D58:D63) + P15*D64)/7</f>
-        <v>10040.564285714285</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+        <v>401.67142857142852</v>
+      </c>
+      <c r="Q11" s="2">
+        <f>(SUM(D58:D60)*Q15 + SUM(D61:D63)*(1/Q15))/6</f>
+        <v>403.55909090909091</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -1175,47 +1236,51 @@
         <v>12</v>
       </c>
       <c r="D12">
-        <v>3356</v>
+        <v>603</v>
       </c>
       <c r="E12">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F12">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G12">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H12">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I12">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J12">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
       <c r="L12" s="7">
         <v>10</v>
       </c>
       <c r="M12" s="3">
         <f>SUM(D65:D70)/6</f>
-        <v>3431.1666666666665</v>
+        <v>894.66666666666663</v>
       </c>
       <c r="N12" s="3">
         <f>(SUM(D65:D67)+MAX(D68:D70))/4</f>
-        <v>3428.75</v>
+        <v>870.5</v>
       </c>
       <c r="O12" s="3">
         <f>(SUM(D65:D68)+AVERAGE(D68,D69)+AVERAGE(D68,D70))/6</f>
-        <v>3432.5</v>
+        <v>872.83333333333337</v>
       </c>
       <c r="P12" s="3">
         <f>(SUM(D65:D70) + P15*D71)/7</f>
-        <v>3454.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+        <v>921.48571428571427</v>
+      </c>
+      <c r="Q12" s="2">
+        <f>(SUM(D65:D67)*Q15 + SUM(D68:D70)*(1/Q15))/6</f>
+        <v>891.9878787878788</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1226,43 +1291,48 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>3338</v>
+        <v>523</v>
       </c>
       <c r="E13">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F13">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G13">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H13">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I13">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J13">
-        <v>7.1999999999998181</v>
-      </c>
-      <c r="L13" s="8" t="s">
+        <v>62.6</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="9">
+      <c r="M13" s="12"/>
+      <c r="N13" s="8">
         <f>(SUM(M3:M12) - SUM(N3:N12)) / COUNT(L3:L12)</f>
-        <v>-1.7</v>
-      </c>
-      <c r="O13" s="9">
+        <v>-14.083333333333394</v>
+      </c>
+      <c r="O13" s="8">
         <f>(SUM(M3:M12) - SUM(O3:O12)) / COUNT(L3:L12)</f>
-        <v>-1.1833333333343035</v>
-      </c>
-      <c r="P13" s="9">
+        <v>7.0333333333332577</v>
+      </c>
+      <c r="P13" s="8">
         <f>(SUM(M3:M12) - SUM(P3:P12)) / COUNT(L3:L12)</f>
-        <v>-40.683571428571305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>-7.5390476190476878</v>
+      </c>
+      <c r="Q13" s="8">
+        <f>(SUM(M3:M12) - SUM(Q3:Q12)) / COUNT(L3:L12)</f>
+        <v>-1.5957575757576705</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1273,31 +1343,34 @@
         <v>14</v>
       </c>
       <c r="D14">
-        <v>3354</v>
+        <v>633</v>
       </c>
       <c r="E14">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F14">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G14">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H14">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I14">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J14">
-        <v>7.1999999999998181</v>
-      </c>
-      <c r="P14" s="11" t="s">
+        <v>62.6</v>
+      </c>
+      <c r="P14" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q14" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -1308,31 +1381,34 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <v>3353</v>
+        <v>532</v>
       </c>
       <c r="E15">
-        <v>3348</v>
+        <v>612</v>
       </c>
       <c r="F15">
-        <v>-4.3333333333334849</v>
+        <v>67.666666669999998</v>
       </c>
       <c r="G15">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="H15">
-        <v>3347</v>
+        <v>563</v>
       </c>
       <c r="I15">
-        <v>3355</v>
+        <v>618</v>
       </c>
       <c r="J15">
-        <v>7.1999999999998181</v>
-      </c>
-      <c r="P15" s="12">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+        <v>62.6</v>
+      </c>
+      <c r="P15" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1343,25 +1419,25 @@
         <v>9</v>
       </c>
       <c r="D16">
-        <v>4022</v>
+        <v>232</v>
       </c>
       <c r="E16">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G16">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H16">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I16">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J16">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1375,25 +1451,25 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>4017</v>
+        <v>301</v>
       </c>
       <c r="E17">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G17">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H17">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I17">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J17">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1407,25 +1483,25 @@
         <v>11</v>
       </c>
       <c r="D18">
-        <v>4014</v>
+        <v>444</v>
       </c>
       <c r="E18">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G18">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H18">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I18">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J18">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1439,25 +1515,25 @@
         <v>12</v>
       </c>
       <c r="D19">
-        <v>4018</v>
+        <v>404</v>
       </c>
       <c r="E19">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G19">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H19">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I19">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J19">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1471,25 +1547,25 @@
         <v>13</v>
       </c>
       <c r="D20">
-        <v>4010</v>
+        <v>346</v>
       </c>
       <c r="E20">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G20">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H20">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I20">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J20">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1503,25 +1579,25 @@
         <v>14</v>
       </c>
       <c r="D21">
-        <v>4004</v>
+        <v>400</v>
       </c>
       <c r="E21">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G21">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H21">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I21">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J21">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -1535,25 +1611,25 @@
         <v>15</v>
       </c>
       <c r="D22">
-        <v>4019</v>
+        <v>219</v>
       </c>
       <c r="E22">
-        <v>4012</v>
+        <v>327</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <v>-57.666666669999998</v>
       </c>
       <c r="G22">
-        <v>-11</v>
+        <v>-31</v>
       </c>
       <c r="H22">
-        <v>4014</v>
+        <v>375</v>
       </c>
       <c r="I22">
-        <v>4011</v>
+        <v>402</v>
       </c>
       <c r="J22">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1567,25 +1643,25 @@
         <v>9</v>
       </c>
       <c r="D23">
-        <v>9100</v>
+        <v>112</v>
       </c>
       <c r="E23">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F23">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G23">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H23">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I23">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J23">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -1599,25 +1675,25 @@
         <v>10</v>
       </c>
       <c r="D24">
-        <v>9095</v>
+        <v>47</v>
       </c>
       <c r="E24">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F24">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G24">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H24">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I24">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J24">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -1631,25 +1707,25 @@
         <v>11</v>
       </c>
       <c r="D25">
-        <v>9094</v>
+        <v>228</v>
       </c>
       <c r="E25">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F25">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G25">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H25">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I25">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J25">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -1663,25 +1739,25 @@
         <v>12</v>
       </c>
       <c r="D26">
-        <v>9112</v>
+        <v>143</v>
       </c>
       <c r="E26">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F26">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G26">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H26">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I26">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J26">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -1695,25 +1771,25 @@
         <v>13</v>
       </c>
       <c r="D27">
-        <v>9096</v>
+        <v>37</v>
       </c>
       <c r="E27">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F27">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G27">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H27">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I27">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J27">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -1727,25 +1803,25 @@
         <v>14</v>
       </c>
       <c r="D28">
-        <v>9092</v>
+        <v>33</v>
       </c>
       <c r="E28">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F28">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G28">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H28">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I28">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J28">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -1759,25 +1835,25 @@
         <v>15</v>
       </c>
       <c r="D29">
-        <v>9102</v>
+        <v>219</v>
       </c>
       <c r="E29">
-        <v>9103</v>
+        <v>120</v>
       </c>
       <c r="F29">
-        <v>-3.6666666666660599</v>
+        <v>58</v>
       </c>
       <c r="G29">
-        <v>-18</v>
+        <v>-108</v>
       </c>
       <c r="H29">
-        <v>9104</v>
+        <v>90</v>
       </c>
       <c r="I29">
-        <v>9102</v>
+        <v>88</v>
       </c>
       <c r="J29">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -1791,25 +1867,25 @@
         <v>9</v>
       </c>
       <c r="D30">
-        <v>9086</v>
+        <v>82</v>
       </c>
       <c r="E30">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F30">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G30">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H30">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I30">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J30">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -1823,25 +1899,25 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>9078</v>
+        <v>84</v>
       </c>
       <c r="E31">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F31">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G31">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H31">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I31">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J31">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -1855,25 +1931,25 @@
         <v>11</v>
       </c>
       <c r="D32">
-        <v>9076</v>
+        <v>284</v>
       </c>
       <c r="E32">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F32">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G32">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H32">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I32">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J32">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -1887,25 +1963,25 @@
         <v>12</v>
       </c>
       <c r="D33">
-        <v>9083</v>
+        <v>161</v>
       </c>
       <c r="E33">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F33">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G33">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H33">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I33">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J33">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -1919,25 +1995,25 @@
         <v>13</v>
       </c>
       <c r="D34">
-        <v>9077</v>
+        <v>219</v>
       </c>
       <c r="E34">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F34">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G34">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H34">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I34">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J34">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -1951,25 +2027,25 @@
         <v>14</v>
       </c>
       <c r="D35">
-        <v>9073</v>
+        <v>313</v>
       </c>
       <c r="E35">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F35">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G35">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H35">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I35">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J35">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -1983,25 +2059,25 @@
         <v>15</v>
       </c>
       <c r="D36">
-        <v>9065</v>
+        <v>111</v>
       </c>
       <c r="E36">
-        <v>9075</v>
+        <v>204</v>
       </c>
       <c r="F36">
-        <v>2.3333333333339401</v>
+        <v>-81</v>
       </c>
       <c r="G36">
-        <v>-8</v>
+        <v>105</v>
       </c>
       <c r="H36">
-        <v>9080</v>
+        <v>190</v>
       </c>
       <c r="I36">
-        <v>9078</v>
+        <v>237</v>
       </c>
       <c r="J36">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -2015,25 +2091,25 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <v>2815</v>
+        <v>454</v>
       </c>
       <c r="E37">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F37">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G37">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H37">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I37">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J37">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -2047,25 +2123,25 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>2808</v>
+        <v>586</v>
       </c>
       <c r="E38">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F38">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G38">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H38">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I38">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J38">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -2079,25 +2155,25 @@
         <v>11</v>
       </c>
       <c r="D39">
-        <v>2817</v>
+        <v>585</v>
       </c>
       <c r="E39">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F39">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G39">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H39">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I39">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J39">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -2111,25 +2187,25 @@
         <v>12</v>
       </c>
       <c r="D40">
-        <v>2820</v>
+        <v>503</v>
       </c>
       <c r="E40">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F40">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G40">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H40">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I40">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J40">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -2143,25 +2219,25 @@
         <v>13</v>
       </c>
       <c r="D41">
-        <v>2804</v>
+        <v>669</v>
       </c>
       <c r="E41">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F41">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G41">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H41">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I41">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J41">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -2175,25 +2251,25 @@
         <v>14</v>
       </c>
       <c r="D42">
-        <v>2802</v>
+        <v>557</v>
       </c>
       <c r="E42">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F42">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G42">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H42">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I42">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J42">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -2207,25 +2283,25 @@
         <v>15</v>
       </c>
       <c r="D43">
-        <v>2803</v>
+        <v>465</v>
       </c>
       <c r="E43">
-        <v>2812</v>
+        <v>545</v>
       </c>
       <c r="F43">
-        <v>4.6666666666669698</v>
+        <v>-34.666666669999998</v>
       </c>
       <c r="G43">
-        <v>-17</v>
+        <v>110</v>
       </c>
       <c r="H43">
-        <v>2812</v>
+        <v>586</v>
       </c>
       <c r="I43">
-        <v>2811</v>
+        <v>530</v>
       </c>
       <c r="J43">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -2239,25 +2315,25 @@
         <v>9</v>
       </c>
       <c r="D44">
-        <v>9195</v>
+        <v>198</v>
       </c>
       <c r="E44">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F44">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G44">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H44">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I44">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J44">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -2271,25 +2347,25 @@
         <v>10</v>
       </c>
       <c r="D45">
-        <v>9199</v>
+        <v>217</v>
       </c>
       <c r="E45">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F45">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G45">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H45">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I45">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J45">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -2303,25 +2379,25 @@
         <v>11</v>
       </c>
       <c r="D46">
-        <v>9182</v>
+        <v>50</v>
       </c>
       <c r="E46">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F46">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G46">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H46">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I46">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J46">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -2335,25 +2411,25 @@
         <v>12</v>
       </c>
       <c r="D47">
-        <v>9200</v>
+        <v>85</v>
       </c>
       <c r="E47">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F47">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G47">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H47">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I47">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J47">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -2367,25 +2443,25 @@
         <v>13</v>
       </c>
       <c r="D48">
-        <v>9190</v>
+        <v>297</v>
       </c>
       <c r="E48">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F48">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G48">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H48">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I48">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J48">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -2399,25 +2475,25 @@
         <v>14</v>
       </c>
       <c r="D49">
-        <v>9192</v>
+        <v>249</v>
       </c>
       <c r="E49">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F49">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G49">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H49">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I49">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J49">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -2431,25 +2507,25 @@
         <v>15</v>
       </c>
       <c r="D50">
-        <v>9197</v>
+        <v>229</v>
       </c>
       <c r="E50">
-        <v>9191</v>
+        <v>175</v>
       </c>
       <c r="F50">
-        <v>-2</v>
+        <v>-55.333333330000002</v>
       </c>
       <c r="G50">
-        <v>-9</v>
+        <v>188</v>
       </c>
       <c r="H50">
-        <v>9195</v>
+        <v>191</v>
       </c>
       <c r="I50">
-        <v>9196</v>
+        <v>167</v>
       </c>
       <c r="J50">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -2463,25 +2539,25 @@
         <v>9</v>
       </c>
       <c r="D51">
-        <v>9396</v>
+        <v>122</v>
       </c>
       <c r="E51">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F51">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G51">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H51">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I51">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J51">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -2495,25 +2571,25 @@
         <v>10</v>
       </c>
       <c r="D52">
-        <v>9406</v>
+        <v>90</v>
       </c>
       <c r="E52">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F52">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G52">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H52">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I52">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J52">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -2527,25 +2603,25 @@
         <v>11</v>
       </c>
       <c r="D53">
-        <v>9408</v>
+        <v>215</v>
       </c>
       <c r="E53">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F53">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G53">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H53">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I53">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J53">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -2559,25 +2635,25 @@
         <v>12</v>
       </c>
       <c r="D54">
-        <v>9391</v>
+        <v>34</v>
       </c>
       <c r="E54">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F54">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G54">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H54">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I54">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J54">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -2591,25 +2667,25 @@
         <v>13</v>
       </c>
       <c r="D55">
-        <v>9399</v>
+        <v>22</v>
       </c>
       <c r="E55">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F55">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G55">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H55">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I55">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J55">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2623,25 +2699,25 @@
         <v>14</v>
       </c>
       <c r="D56">
-        <v>9405</v>
+        <v>118</v>
       </c>
       <c r="E56">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F56">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G56">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H56">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I56">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J56">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -2655,25 +2731,25 @@
         <v>15</v>
       </c>
       <c r="D57">
-        <v>9394</v>
+        <v>206</v>
       </c>
       <c r="E57">
-        <v>9401</v>
+        <v>136</v>
       </c>
       <c r="F57">
-        <v>5</v>
+        <v>84.333333330000002</v>
       </c>
       <c r="G57">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="H57">
-        <v>9395</v>
+        <v>28</v>
       </c>
       <c r="I57">
-        <v>9398</v>
+        <v>76</v>
       </c>
       <c r="J57">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -2687,25 +2763,25 @@
         <v>9</v>
       </c>
       <c r="D58">
-        <v>9966</v>
+        <v>355</v>
       </c>
       <c r="E58">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F58">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G58">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H58">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I58">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J58">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
@@ -2719,25 +2795,25 @@
         <v>10</v>
       </c>
       <c r="D59">
-        <v>9965</v>
+        <v>527</v>
       </c>
       <c r="E59">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F59">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G59">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H59">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I59">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J59">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -2751,25 +2827,25 @@
         <v>11</v>
       </c>
       <c r="D60">
-        <v>9976</v>
+        <v>387</v>
       </c>
       <c r="E60">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F60">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G60">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H60">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I60">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J60">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -2783,25 +2859,25 @@
         <v>12</v>
       </c>
       <c r="D61">
-        <v>9961</v>
+        <v>336</v>
       </c>
       <c r="E61">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F61">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G61">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H61">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I61">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J61">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -2815,25 +2891,25 @@
         <v>13</v>
       </c>
       <c r="D62">
-        <v>9963</v>
+        <v>340</v>
       </c>
       <c r="E62">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F62">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G62">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H62">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I62">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J62">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -2847,25 +2923,25 @@
         <v>14</v>
       </c>
       <c r="D63">
-        <v>9975</v>
+        <v>452</v>
       </c>
       <c r="E63">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F63">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G63">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H63">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I63">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J63">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -2879,25 +2955,25 @@
         <v>15</v>
       </c>
       <c r="D64">
-        <v>9979</v>
+        <v>377</v>
       </c>
       <c r="E64">
-        <v>9970</v>
+        <v>417</v>
       </c>
       <c r="F64">
-        <v>2.6666666666660599</v>
+        <v>47</v>
       </c>
       <c r="G64">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H64">
-        <v>9962</v>
+        <v>338</v>
       </c>
       <c r="I64">
-        <v>9968</v>
+        <v>394</v>
       </c>
       <c r="J64">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
@@ -2911,25 +2987,25 @@
         <v>9</v>
       </c>
       <c r="D65">
-        <v>3422</v>
+        <v>851</v>
       </c>
       <c r="E65">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F65">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G65">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H65">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I65">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J65">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -2943,25 +3019,25 @@
         <v>10</v>
       </c>
       <c r="D66">
-        <v>3428</v>
+        <v>834</v>
       </c>
       <c r="E66">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F66">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G66">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H66">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I66">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J66">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -2975,25 +3051,25 @@
         <v>11</v>
       </c>
       <c r="D67">
-        <v>3421</v>
+        <v>787</v>
       </c>
       <c r="E67">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F67">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G67">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H67">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I67">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J67">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -3007,25 +3083,25 @@
         <v>12</v>
       </c>
       <c r="D68">
-        <v>3444</v>
+        <v>878</v>
       </c>
       <c r="E68">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F68">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G68">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H68">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I68">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J68">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
@@ -3039,25 +3115,25 @@
         <v>13</v>
       </c>
       <c r="D69">
-        <v>3440</v>
+        <v>1010</v>
       </c>
       <c r="E69">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F69">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G69">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H69">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I69">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J69">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
@@ -3071,25 +3147,25 @@
         <v>14</v>
       </c>
       <c r="D70">
-        <v>3432</v>
+        <v>1008</v>
       </c>
       <c r="E70">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F70">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G70">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H70">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I70">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J70">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -3103,28 +3179,31 @@
         <v>15</v>
       </c>
       <c r="D71">
-        <v>3424</v>
+        <v>984</v>
       </c>
       <c r="E71">
-        <v>3432</v>
+        <v>890</v>
       </c>
       <c r="F71">
-        <v>-15</v>
+        <v>-141.33333329999999</v>
       </c>
       <c r="G71">
-        <v>-8</v>
+        <v>131</v>
       </c>
       <c r="H71">
-        <v>3442</v>
+        <v>944</v>
       </c>
       <c r="I71">
-        <v>3438</v>
+        <v>943</v>
       </c>
       <c r="J71">
-        <v>7.1999999999998181</v>
+        <v>62.6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L13:M13"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>